<commit_message>
10 Non Working Days
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Loan Product/4615-WorkingNoNWorking-Loanproduct.xlsx
+++ b/Mifos Automation Excels/Loan Product/4615-WorkingNoNWorking-Loanproduct.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>productname</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>startdate</t>
   </si>
   <si>
     <t>includeincustomerloancounter</t>
@@ -117,10 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\-mmmm\-yyyy"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,12 +122,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -175,14 +163,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -194,7 +179,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,184 +481,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>30</v>
+      <c r="B1" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>4615</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>4615</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
-        <v>41275</v>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="9" t="s">
         <v>14</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="12" t="s">
         <v>28</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="B20" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -697,11 +674,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>24</v>
+      <c r="A1" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>